<commit_message>
Added some few files
</commit_message>
<xml_diff>
--- a/unifiedSettings_ui/TestData/TestCases.xlsx
+++ b/unifiedSettings_ui/TestData/TestCases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D38D5A-2F30-4AB3-B485-54A8FB8E0AEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{288402DA-0E67-41E2-84A2-8C6C3721A86F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="29070" windowHeight="16500" tabRatio="935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="UnmanagedProspects" sheetId="19" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K8"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -1059,7 +1060,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2024,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>